<commit_message>
feat: Update Issue 3 (Product dan Sales, Daily Audit Not Finished Yet)
</commit_message>
<xml_diff>
--- a/public/template/report/Template_Report_Product_Low_Stock.xlsx
+++ b/public/template/report/Template_Report_Product_Low_Stock.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9F6E19-8459-4856-84D5-657F260B6C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEA0764-E11D-4382-B731-5CB2E8703E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Report Product Low Stock" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="999999"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -37,7 +37,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Low Stock</t>
+    <t>In-Stock</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>